<commit_message>
Support generated dataset and HTML report
</commit_message>
<xml_diff>
--- a/examples/official/zxing_zbar/benchmark.xlsx
+++ b/examples/official/zxing_zbar/benchmark.xlsx
@@ -1215,7 +1215,11 @@
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr"/>
-      <c r="D32" s="2" t="inlineStr"/>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>2494593028073</t>
+        </is>
+      </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
           <t>2494593028073</t>
@@ -1437,9 +1441,9 @@
           <t>3222476758729</t>
         </is>
       </c>
-      <c r="D42" s="1" t="inlineStr">
-        <is>
-          <t>3222476758729</t>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>12221701</t>
         </is>
       </c>
       <c r="E42" s="2" t="inlineStr"/>
@@ -1483,7 +1487,11 @@
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr"/>
-      <c r="D44" s="2" t="inlineStr"/>
+      <c r="D44" s="1" t="inlineStr">
+        <is>
+          <t>3240931541419</t>
+        </is>
+      </c>
       <c r="E44" s="2" t="inlineStr"/>
     </row>
     <row r="45">
@@ -2267,7 +2275,11 @@
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr"/>
-      <c r="D76" s="2" t="inlineStr"/>
+      <c r="D76" s="1" t="inlineStr">
+        <is>
+          <t>3425470021008</t>
+        </is>
+      </c>
       <c r="E76" s="2" t="inlineStr"/>
     </row>
     <row r="77">
@@ -2282,7 +2294,11 @@
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr"/>
-      <c r="D77" s="2" t="inlineStr"/>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>2600185021586</t>
+        </is>
+      </c>
       <c r="E77" s="2" t="inlineStr"/>
     </row>
     <row r="78">
@@ -2324,7 +2340,11 @@
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr"/>
-      <c r="D79" s="2" t="inlineStr"/>
+      <c r="D79" s="1" t="inlineStr">
+        <is>
+          <t>3448550008010</t>
+        </is>
+      </c>
       <c r="E79" s="2" t="inlineStr"/>
     </row>
     <row r="80">
@@ -2665,7 +2685,11 @@
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr"/>
-      <c r="D94" s="2" t="inlineStr"/>
+      <c r="D94" s="1" t="inlineStr">
+        <is>
+          <t>3560071094980</t>
+        </is>
+      </c>
       <c r="E94" s="2" t="inlineStr"/>
     </row>
     <row r="95">
@@ -3468,7 +3492,11 @@
         </is>
       </c>
       <c r="C127" s="2" t="inlineStr"/>
-      <c r="D127" s="2" t="inlineStr"/>
+      <c r="D127" s="1" t="inlineStr">
+        <is>
+          <t>4250665325581</t>
+        </is>
+      </c>
       <c r="E127" s="2" t="inlineStr"/>
     </row>
     <row r="128">
@@ -3648,7 +3676,11 @@
           <t>4311501625217</t>
         </is>
       </c>
-      <c r="D135" s="2" t="inlineStr"/>
+      <c r="D135" s="1" t="inlineStr">
+        <is>
+          <t>4311501625217</t>
+        </is>
+      </c>
       <c r="E135" s="2" t="inlineStr"/>
     </row>
     <row r="136">
@@ -4539,7 +4571,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>87.06%</t>
+          <t>90.59%</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">

</xml_diff>